<commit_message>
Update Projektbudget.tex Besprochene Zeiten eingefügt
</commit_message>
<xml_diff>
--- a/Pflichtenheft/Ext. files/Projektstrukturplan+Budget.xlsx
+++ b/Pflichtenheft/Ext. files/Projektstrukturplan+Budget.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\OneDrive\Dokumente\GitHub\Pro1E\Pflichtenheft\Ext. files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lars\Documents\GitHub\Pro1\Pflichtenheft\Ext. files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="13_ncr:9_{7A03DF05-4470-4A34-BCAD-3BC6EBE3C1B1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{71E73C56-42E0-49A3-91AF-B0F656544972}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3247D432-08BD-4D28-8AA0-14EA0D85129F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7870" activeTab="1" xr2:uid="{87A0319D-F60A-4D81-9B19-F1322DFC7471}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7875" firstSheet="1" activeTab="1" xr2:uid="{87A0319D-F60A-4D81-9B19-F1322DFC7471}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektstrukturplan" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
   <si>
     <t>Projektstrukturplan</t>
   </si>
@@ -986,6 +986,9 @@
   </si>
   <si>
     <t>6. Reserve</t>
+  </si>
+  <si>
+    <t>NICHT AKTUELL!!!</t>
   </si>
 </sst>
 </file>
@@ -994,9 +997,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_ &quot;CHF&quot;\ * #,##0.00_ ;_ &quot;CHF&quot;\ * \-#,##0.00_ ;_ &quot;CHF&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +1039,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1139,7 +1150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1208,9 +1219,10 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1525,20 +1537,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7216B3FB-D6CA-4A11-8540-8FD01F7DF887}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.1796875" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,8 +1561,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D1" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1559,7 +1575,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1569,7 +1585,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1580,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1591,7 +1607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1602,7 +1618,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -1612,7 +1628,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1623,7 +1639,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -1634,7 +1650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1661,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
@@ -1656,7 +1672,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
@@ -1667,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1678,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -1689,7 +1705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
@@ -1700,12 +1716,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="10"/>
     </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1715,7 +1731,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>23</v>
       </c>
@@ -1726,7 +1742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>24</v>
       </c>
@@ -1737,7 +1753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>25</v>
       </c>
@@ -1748,12 +1764,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="9"/>
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>26</v>
       </c>
@@ -1763,7 +1779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
@@ -1774,7 +1790,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1785,7 +1801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -1796,7 +1812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>31</v>
       </c>
@@ -1807,7 +1823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
@@ -1818,12 +1834,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10"/>
     </row>
-    <row r="29" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>33</v>
       </c>
@@ -1833,7 +1849,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>34</v>
       </c>
@@ -1844,7 +1860,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>35</v>
       </c>
@@ -1855,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>36</v>
       </c>
@@ -1866,7 +1882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>37</v>
       </c>
@@ -1877,7 +1893,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>38</v>
       </c>
@@ -1888,12 +1904,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
     </row>
-    <row r="36" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>55</v>
       </c>
@@ -1903,7 +1919,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
@@ -1914,12 +1930,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
     </row>
-    <row r="39" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -1929,7 +1945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>57</v>
       </c>
@@ -1951,26 +1967,26 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>40</v>
       </c>
@@ -1987,7 +2003,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="16" t="s">
         <v>46</v>
       </c>
@@ -1997,103 +2013,99 @@
       </c>
       <c r="D4" s="26">
         <f t="shared" ref="D4:D10" si="0">C4/$C$10</f>
-        <v>0.23178807947019867</v>
+        <v>0.20710059171597633</v>
       </c>
       <c r="E4" s="14">
         <f>C4*74</f>
         <v>7770</v>
       </c>
       <c r="F4" s="26">
-        <f t="shared" ref="F4:F10" si="1">E4/$E$10</f>
-        <v>0.21875</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <f t="shared" ref="F4:F9" si="1">E4/$E$10</f>
+        <v>0.19699812382739212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>47</v>
       </c>
       <c r="C5" s="13">
-        <f>Projektstrukturplan!C17</f>
-        <v>35</v>
+        <v>115</v>
       </c>
       <c r="D5" s="26">
         <f t="shared" si="0"/>
-        <v>7.7262693156732898E-2</v>
+        <v>0.22682445759368836</v>
       </c>
       <c r="E5" s="14">
         <f>C5*74</f>
-        <v>2590</v>
+        <v>8510</v>
       </c>
       <c r="F5" s="26">
         <f t="shared" si="1"/>
-        <v>7.2916666666666671E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.21575984990619138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15"/>
       <c r="B6" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="13">
-        <f>Projektstrukturplan!C22</f>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="26">
         <f t="shared" si="0"/>
-        <v>5.9602649006622516E-2</v>
+        <v>5.128205128205128E-2</v>
       </c>
       <c r="E6" s="14">
         <f>C6*148</f>
-        <v>3996</v>
+        <v>3848</v>
       </c>
       <c r="F6" s="26">
         <f t="shared" si="1"/>
-        <v>0.1125</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>9.7560975609756101E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="13">
-        <f>Projektstrukturplan!C29</f>
-        <v>86</v>
+        <v>121</v>
       </c>
       <c r="D7" s="26">
         <f t="shared" si="0"/>
-        <v>0.18984547461368653</v>
+        <v>0.23865877712031558</v>
       </c>
       <c r="E7" s="14">
         <f>C7*74</f>
-        <v>6364</v>
+        <v>8954</v>
       </c>
       <c r="F7" s="26">
         <f t="shared" si="1"/>
-        <v>0.17916666666666667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.22701688555347091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="13">
-        <f>Projektstrukturplan!C36</f>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="D8" s="26">
         <f t="shared" si="0"/>
-        <v>0.35320088300220753</v>
+        <v>0.19723865877712032</v>
       </c>
       <c r="E8" s="14">
         <f>C8*74</f>
-        <v>11840</v>
+        <v>7400</v>
       </c>
       <c r="F8" s="26">
         <f t="shared" si="1"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>0.18761726078799248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="17" t="s">
         <v>59</v>
       </c>
@@ -2103,7 +2115,7 @@
       </c>
       <c r="D9" s="26">
         <f t="shared" si="0"/>
-        <v>8.8300220750551883E-2</v>
+        <v>7.8895463510848127E-2</v>
       </c>
       <c r="E9" s="14">
         <f>C9*74</f>
@@ -2111,16 +2123,16 @@
       </c>
       <c r="F9" s="26">
         <f t="shared" si="1"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+        <v>7.5046904315197005E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="22">
         <f>SUM(C4:C9)</f>
-        <v>453</v>
+        <v>507</v>
       </c>
       <c r="D10" s="23">
         <f t="shared" si="0"/>
@@ -2128,32 +2140,32 @@
       </c>
       <c r="E10" s="24">
         <f>SUM(E4:E9)</f>
-        <v>35520</v>
+        <v>39442</v>
       </c>
       <c r="F10" s="23">
         <f>SUM(F4:F9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="20">
         <f>E10</f>
-        <v>35520</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>39442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="s">
         <v>50</v>
       </c>
       <c r="C13">
         <f>C10</f>
-        <v>453</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>51</v>
       </c>
@@ -2161,13 +2173,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="19">
         <f>C13/C14</f>
-        <v>75.5</v>
+        <v>84.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>